<commit_message>
writing reshaped data to file so that can be read in instead of reshaping raw results each time
</commit_message>
<xml_diff>
--- a/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
+++ b/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeagueSpark/game-of-thrones-spark/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C0156AAA-1D1F-7C40-BA92-FAC949730263}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A204AE07-B05B-3E45-8875-ADCC9BAC78EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="5060" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="4440" yWindow="5060" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_anne-testing_game_answer_s" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t>questionNumber</t>
   </si>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t>correctAnswer</t>
-  </si>
-  <si>
-    <t>Dies</t>
   </si>
   <si>
     <t>Lives</t>
@@ -346,7 +343,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1188,11 +1185,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1258,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1278,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1298,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1318,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1358,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1378,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1398,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1458,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1478,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1498,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1518,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1538,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1558,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1578,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1598,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1618,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1638,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1658,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1678,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1953,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
week 2 correct answer sheet, changing sign of difference in rank to be positive for lower rank
</commit_message>
<xml_diff>
--- a/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
+++ b/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeagueSpark/game-of-thrones-spark/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A204AE07-B05B-3E45-8875-ADCC9BAC78EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD6BA43-3F34-D544-8D0B-EB7E632B61EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="5060" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t>questionNumber</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>None of the above</t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1998,10 +2001,13 @@
         <v>3</v>
       </c>
       <c r="D43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding yaml config file to store filenames
</commit_message>
<xml_diff>
--- a/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
+++ b/game-of-thrones-spark/src/main/resources/correct_answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeagueSpark/game-of-thrones-spark/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD6BA43-3F34-D544-8D0B-EB7E632B61EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A4E870-E75A-B64F-921D-4A22C8DBA5B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="5060" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7860" yWindow="1660" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_anne-testing_game_answer_s" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
   <si>
     <t>questionNumber</t>
   </si>
@@ -341,6 +341,39 @@
   </si>
   <si>
     <t>None of the above</t>
+  </si>
+  <si>
+    <t>Dies</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Edd Tollett</t>
+  </si>
+  <si>
+    <t>Rhaegal</t>
+  </si>
+  <si>
+    <t>The Hound kills Ser Gregor, Ser Gregor kills Qyburn</t>
+  </si>
+  <si>
+    <t>No One/There will be no Iron Throne</t>
+  </si>
+  <si>
+    <t>There is no prince that was promised</t>
+  </si>
+  <si>
+    <t>Edmure Tully, Robin Arryn</t>
+  </si>
+  <si>
+    <t>Nymeria, Ghost, Drogon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilly and Samwell </t>
+  </si>
+  <si>
+    <t>Arya kills the Night's King</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1258,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1378,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1478,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1518,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1578,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1598,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1658,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1692,10 +1725,13 @@
         <v>6</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1709,10 +1745,13 @@
         <v>4</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1726,10 +1765,13 @@
         <v>5</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1743,10 +1785,13 @@
         <v>2</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1760,10 +1805,13 @@
         <v>4</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1777,10 +1825,13 @@
         <v>4</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1794,10 +1845,13 @@
         <v>2</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1811,10 +1865,13 @@
         <v>1</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1828,10 +1885,13 @@
         <v>1</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1845,10 +1905,13 @@
         <v>1</v>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,10 +1925,13 @@
         <v>1</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1879,10 +1945,13 @@
         <v>1</v>
       </c>
       <c r="D36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,10 +1965,13 @@
         <v>1</v>
       </c>
       <c r="D37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1913,10 +1985,13 @@
         <v>1</v>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1930,10 +2005,13 @@
         <v>1</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1967,10 +2045,13 @@
         <v>1</v>
       </c>
       <c r="D41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1984,10 +2065,13 @@
         <v>2</v>
       </c>
       <c r="D42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2021,10 +2105,13 @@
         <v>2</v>
       </c>
       <c r="D44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2038,10 +2125,13 @@
         <v>2</v>
       </c>
       <c r="D45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2055,10 +2145,13 @@
         <v>2</v>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2072,10 +2165,13 @@
         <v>2</v>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2089,13 +2185,16 @@
         <v>4</v>
       </c>
       <c r="D48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2106,13 +2205,16 @@
         <v>3</v>
       </c>
       <c r="D49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -2125,9 +2227,12 @@
       <c r="E50" t="b">
         <v>0</v>
       </c>
+      <c r="F50">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
     <sortCondition ref="A2:A50"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>